<commit_message>
up des fichiers à modifier
</commit_message>
<xml_diff>
--- a/P4_01_Analyse.xlsx
+++ b/P4_01_Analyse.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
   <si>
     <t>Catégorie</t>
   </si>
@@ -178,6 +178,21 @@
   </si>
   <si>
     <t>Décrire l'image via la balise alt= " "</t>
+  </si>
+  <si>
+    <t>SEO et accessibilité</t>
+  </si>
+  <si>
+    <t>langue non identifié dans le fichier html</t>
+  </si>
+  <si>
+    <t>Toujours indiquer la langue dans un document afin d'atteindre les personnes concerné par cette langue</t>
+  </si>
+  <si>
+    <t>langue non identifié dans le fichier html bloque le bon référencement au près des utilisateurs potentiels, le site peut être proposé auprès  d'utilisateurs non concernés</t>
+  </si>
+  <si>
+    <t>spécifier la langue en utilisant &lt;html lang="fr"&gt;</t>
   </si>
 </sst>
 </file>
@@ -487,7 +502,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -729,7 +744,23 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:26" ht="60" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>